<commit_message>
Fixed 3 uploaded file and added a datatable
</commit_message>
<xml_diff>
--- a/sample csv/test/Copy of F-IVM-008 Weekly Materials Inventory as of October 2024.xlsx
+++ b/sample csv/test/Copy of F-IVM-008 Weekly Materials Inventory as of October 2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chuckie Miras\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xamp\htdocs\inventory_system\sample csv\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CC88BF-934B-4B5F-BC58-A895A1B5370B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D06B3BE-DB46-4B6F-A4E4-A40802F4DB4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BA3C271-9574-45E1-A861-C71CBF0E9786}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BA3C271-9574-45E1-A861-C71CBF0E9786}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,22 +263,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974E1216-3E72-4D54-BF9B-B1F971E61FE3}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,26 +620,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
@@ -649,18 +649,18 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -668,20 +668,20 @@
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">

</xml_diff>